<commit_message>
Finally have an actual player rankings list!
</commit_message>
<xml_diff>
--- a/testseason.xlsx
+++ b/testseason.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9450" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9450" firstSheet="6" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team Info" sheetId="1" r:id="rId1"/>
@@ -801,9 +801,6 @@
     <t>Henry Prosser</t>
   </si>
   <si>
-    <t>Aidan daly-Jensen</t>
-  </si>
-  <si>
     <t>Clark Fisher</t>
   </si>
   <si>
@@ -1420,6 +1417,9 @@
   </si>
   <si>
     <t>Gugliemo Carcano</t>
+  </si>
+  <si>
+    <t>Aidan Daly-Jensen</t>
   </si>
 </sst>
 </file>
@@ -2199,25 +2199,25 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -2225,25 +2225,25 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="G12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -2251,25 +2251,25 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K13" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -2277,25 +2277,25 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="K14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -2303,25 +2303,25 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -2329,25 +2329,25 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
+        <v>280</v>
+      </c>
+      <c r="D16" t="s">
+        <v>280</v>
+      </c>
+      <c r="E16" t="s">
+        <v>280</v>
+      </c>
+      <c r="F16" t="s">
         <v>281</v>
       </c>
-      <c r="D16" t="s">
-        <v>281</v>
-      </c>
-      <c r="E16" t="s">
-        <v>281</v>
-      </c>
-      <c r="F16" t="s">
-        <v>282</v>
-      </c>
       <c r="G16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K16" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -2355,25 +2355,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F17" t="s">
+        <v>280</v>
+      </c>
+      <c r="G17" t="s">
         <v>281</v>
       </c>
-      <c r="G17" t="s">
-        <v>282</v>
-      </c>
       <c r="I17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K17" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -2381,25 +2381,25 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I18" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -2407,25 +2407,25 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -2899,25 +2899,25 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I11" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2925,25 +2925,25 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I12" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2951,25 +2951,25 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2977,25 +2977,25 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3003,25 +3003,25 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3029,25 +3029,25 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E16" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -3055,25 +3055,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F17" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -3081,25 +3081,25 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -3107,25 +3107,25 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="G19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -3574,16 +3574,16 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G11" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -3608,16 +3608,16 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -3625,16 +3625,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="G14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3659,16 +3659,16 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -3676,16 +3676,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -3693,16 +3693,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -4192,28 +4192,28 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -4221,28 +4221,28 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -4250,28 +4250,28 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G13" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -4279,28 +4279,28 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -4308,28 +4308,28 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -4337,28 +4337,28 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
+        <v>319</v>
+      </c>
+      <c r="D16" t="s">
+        <v>319</v>
+      </c>
+      <c r="E16" t="s">
+        <v>319</v>
+      </c>
+      <c r="F16" t="s">
+        <v>319</v>
+      </c>
+      <c r="G16" t="s">
+        <v>316</v>
+      </c>
+      <c r="H16" t="s">
         <v>320</v>
       </c>
-      <c r="D16" t="s">
+      <c r="I16" t="s">
         <v>320</v>
       </c>
-      <c r="E16" t="s">
+      <c r="J16" t="s">
         <v>320</v>
-      </c>
-      <c r="F16" t="s">
-        <v>320</v>
-      </c>
-      <c r="G16" t="s">
-        <v>317</v>
-      </c>
-      <c r="H16" t="s">
-        <v>321</v>
-      </c>
-      <c r="I16" t="s">
-        <v>321</v>
-      </c>
-      <c r="J16" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -4366,28 +4366,28 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" t="s">
+        <v>320</v>
+      </c>
+      <c r="E17" t="s">
+        <v>320</v>
+      </c>
+      <c r="F17" t="s">
+        <v>320</v>
+      </c>
+      <c r="G17" t="s">
+        <v>323</v>
+      </c>
+      <c r="H17" t="s">
+        <v>319</v>
+      </c>
+      <c r="I17" t="s">
+        <v>319</v>
+      </c>
+      <c r="J17" t="s">
         <v>321</v>
-      </c>
-      <c r="D17" t="s">
-        <v>321</v>
-      </c>
-      <c r="E17" t="s">
-        <v>321</v>
-      </c>
-      <c r="F17" t="s">
-        <v>321</v>
-      </c>
-      <c r="G17" t="s">
-        <v>324</v>
-      </c>
-      <c r="H17" t="s">
-        <v>320</v>
-      </c>
-      <c r="I17" t="s">
-        <v>320</v>
-      </c>
-      <c r="J17" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -4395,28 +4395,28 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
+        <v>321</v>
+      </c>
+      <c r="D18" t="s">
+        <v>321</v>
+      </c>
+      <c r="E18" t="s">
+        <v>321</v>
+      </c>
+      <c r="F18" t="s">
+        <v>316</v>
+      </c>
+      <c r="G18" t="s">
+        <v>319</v>
+      </c>
+      <c r="H18" t="s">
         <v>322</v>
       </c>
-      <c r="D18" t="s">
+      <c r="I18" t="s">
         <v>322</v>
       </c>
-      <c r="E18" t="s">
+      <c r="J18" t="s">
         <v>322</v>
-      </c>
-      <c r="F18" t="s">
-        <v>317</v>
-      </c>
-      <c r="G18" t="s">
-        <v>320</v>
-      </c>
-      <c r="H18" t="s">
-        <v>323</v>
-      </c>
-      <c r="I18" t="s">
-        <v>323</v>
-      </c>
-      <c r="J18" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -4424,28 +4424,28 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -4949,22 +4949,22 @@
         <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -4972,22 +4972,22 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I12" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -4995,22 +4995,22 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I13" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -5018,22 +5018,22 @@
         <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -5041,22 +5041,22 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -5064,22 +5064,22 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="H16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I16" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -5087,22 +5087,22 @@
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="H17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I17" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -5110,22 +5110,22 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -5133,22 +5133,22 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -5621,7 +5621,7 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -5629,7 +5629,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -5637,7 +5637,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5645,7 +5645,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -5653,7 +5653,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -5661,7 +5661,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -5669,7 +5669,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -5677,7 +5677,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -5685,7 +5685,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -6784,28 +6784,28 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="F11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="I11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -6813,28 +6813,28 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="I12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K12" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -6842,28 +6842,28 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -6871,28 +6871,28 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -6900,28 +6900,28 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="I15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -6929,28 +6929,28 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="I16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -6958,28 +6958,28 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="I17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K17" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -6987,28 +6987,28 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
+        <v>350</v>
+      </c>
+      <c r="D18" t="s">
+        <v>350</v>
+      </c>
+      <c r="E18" t="s">
+        <v>350</v>
+      </c>
+      <c r="F18" t="s">
+        <v>350</v>
+      </c>
+      <c r="G18" t="s">
         <v>351</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
         <v>351</v>
       </c>
-      <c r="E18" t="s">
+      <c r="I18" t="s">
         <v>351</v>
       </c>
-      <c r="F18" t="s">
-        <v>351</v>
-      </c>
-      <c r="G18" t="s">
-        <v>352</v>
-      </c>
-      <c r="H18" t="s">
-        <v>352</v>
-      </c>
-      <c r="I18" t="s">
-        <v>352</v>
-      </c>
       <c r="K18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -7016,28 +7016,28 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G19" t="s">
+        <v>350</v>
+      </c>
+      <c r="H19" t="s">
+        <v>350</v>
+      </c>
+      <c r="I19" t="s">
+        <v>350</v>
+      </c>
+      <c r="K19" t="s">
         <v>351</v>
-      </c>
-      <c r="H19" t="s">
-        <v>351</v>
-      </c>
-      <c r="I19" t="s">
-        <v>351</v>
-      </c>
-      <c r="K19" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -7486,16 +7486,16 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G11" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -7503,16 +7503,16 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="G12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -7520,16 +7520,16 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G13" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -7537,16 +7537,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="G14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -7554,16 +7554,16 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G15" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -7571,16 +7571,16 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -7588,16 +7588,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="G17" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -7605,16 +7605,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="G18" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -7622,16 +7622,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="G19" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -8151,28 +8151,28 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H11" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="I11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="J11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -8180,28 +8180,28 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H12" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J12" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -8209,28 +8209,28 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="I13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="J13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -8238,28 +8238,28 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="I14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -8267,28 +8267,28 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="J15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -8296,28 +8296,28 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
+        <v>358</v>
+      </c>
+      <c r="D16" t="s">
+        <v>357</v>
+      </c>
+      <c r="E16" t="s">
+        <v>357</v>
+      </c>
+      <c r="F16" t="s">
+        <v>357</v>
+      </c>
+      <c r="G16" t="s">
         <v>359</v>
       </c>
-      <c r="D16" t="s">
-        <v>358</v>
-      </c>
-      <c r="E16" t="s">
-        <v>358</v>
-      </c>
-      <c r="F16" t="s">
-        <v>358</v>
-      </c>
-      <c r="G16" t="s">
-        <v>360</v>
-      </c>
       <c r="H16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="J16" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -8325,28 +8325,28 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>359</v>
+      </c>
+      <c r="D17" t="s">
         <v>360</v>
       </c>
-      <c r="D17" t="s">
-        <v>361</v>
-      </c>
       <c r="E17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="J17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -8354,28 +8354,28 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H18" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -8383,28 +8383,28 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J19" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -8666,8 +8666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8772,7 +8772,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="1">
-        <v>42155</v>
+        <v>42156</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -8783,7 +8783,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1">
-        <v>42141</v>
+        <v>42157</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -8794,7 +8794,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>42092</v>
+        <v>42158</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -8805,7 +8805,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="1">
-        <v>42093</v>
+        <v>42159</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -8816,7 +8816,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="1">
-        <v>42095</v>
+        <v>42160</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -8827,7 +8827,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="1">
-        <v>42096</v>
+        <v>42161</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -8838,7 +8838,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="1">
-        <v>42097</v>
+        <v>42162</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -8849,7 +8849,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="1">
-        <v>42098</v>
+        <v>42163</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -8860,7 +8860,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="1">
-        <v>42099</v>
+        <v>42164</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -8871,7 +8871,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="1">
-        <v>42100</v>
+        <v>42165</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8882,7 +8882,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="1">
-        <v>42101</v>
+        <v>42166</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -8893,7 +8893,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="1">
-        <v>42102</v>
+        <v>42167</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -8904,7 +8904,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="1">
-        <v>42103</v>
+        <v>42168</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -8915,7 +8915,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="1">
-        <v>42104</v>
+        <v>42169</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -9073,16 +9073,16 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F11" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -9090,16 +9090,16 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E12" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -9107,16 +9107,16 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
+        <v>373</v>
+      </c>
+      <c r="D13" t="s">
         <v>374</v>
       </c>
-      <c r="D13" t="s">
-        <v>375</v>
-      </c>
       <c r="E13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -9124,16 +9124,16 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -9141,16 +9141,16 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -9158,16 +9158,16 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
+        <v>376</v>
+      </c>
+      <c r="D16" t="s">
         <v>377</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
+        <v>377</v>
+      </c>
+      <c r="F16" t="s">
         <v>378</v>
-      </c>
-      <c r="E16" t="s">
-        <v>378</v>
-      </c>
-      <c r="F16" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -9175,16 +9175,16 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
+        <v>377</v>
+      </c>
+      <c r="D17" t="s">
         <v>378</v>
       </c>
-      <c r="D17" t="s">
-        <v>379</v>
-      </c>
       <c r="E17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -9192,16 +9192,16 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
+        <v>378</v>
+      </c>
+      <c r="D18" t="s">
         <v>379</v>
       </c>
-      <c r="D18" t="s">
-        <v>380</v>
-      </c>
       <c r="E18" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -9209,16 +9209,16 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F19" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -9701,25 +9701,25 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -9727,25 +9727,25 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -9753,25 +9753,25 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -9779,25 +9779,25 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -9805,25 +9805,25 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K15" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -9831,25 +9831,25 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F16" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="K16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
@@ -9857,25 +9857,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -9883,25 +9883,25 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -9912,22 +9912,22 @@
         <v>14</v>
       </c>
       <c r="D19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -10389,19 +10389,19 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H11" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10409,19 +10409,19 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G12" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H12" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -10429,19 +10429,19 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D13" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H13" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -10449,19 +10449,19 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="G14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10469,19 +10469,19 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D15" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -10489,19 +10489,19 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D16" t="s">
+        <v>452</v>
+      </c>
+      <c r="F16" t="s">
         <v>453</v>
       </c>
-      <c r="F16" t="s">
-        <v>454</v>
-      </c>
       <c r="G16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H16" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -10509,19 +10509,19 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G17" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H17" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -10529,19 +10529,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="G18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H18" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -10549,19 +10549,19 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D19" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="G19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -11073,22 +11073,22 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="J11" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -11096,22 +11096,22 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="J12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -11119,22 +11119,22 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E13" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -11142,22 +11142,22 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -11165,22 +11165,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D15" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G15" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="J15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -11188,22 +11188,22 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E16" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="J16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
@@ -11211,22 +11211,22 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -11234,22 +11234,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E18" t="s">
+        <v>396</v>
+      </c>
+      <c r="F18" t="s">
+        <v>398</v>
+      </c>
+      <c r="G18" t="s">
         <v>397</v>
       </c>
-      <c r="F18" t="s">
-        <v>399</v>
-      </c>
-      <c r="G18" t="s">
-        <v>398</v>
-      </c>
       <c r="J18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
@@ -11257,22 +11257,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E19" t="s">
+        <v>397</v>
+      </c>
+      <c r="F19" t="s">
+        <v>397</v>
+      </c>
+      <c r="G19" t="s">
         <v>398</v>
       </c>
-      <c r="F19" t="s">
-        <v>398</v>
-      </c>
-      <c r="G19" t="s">
-        <v>399</v>
-      </c>
       <c r="J19" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -11739,22 +11739,22 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -11762,22 +11762,22 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -11785,22 +11785,22 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -11808,22 +11808,22 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -11831,22 +11831,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
+        <v>409</v>
+      </c>
+      <c r="D15" t="s">
         <v>410</v>
       </c>
-      <c r="D15" t="s">
-        <v>411</v>
-      </c>
       <c r="E15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -11854,22 +11854,22 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -11877,22 +11877,22 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -11900,22 +11900,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -11923,22 +11923,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D19" t="s">
+        <v>414</v>
+      </c>
+      <c r="E19" t="s">
+        <v>414</v>
+      </c>
+      <c r="F19" t="s">
         <v>415</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>415</v>
       </c>
-      <c r="F19" t="s">
-        <v>416</v>
-      </c>
-      <c r="G19" t="s">
-        <v>416</v>
-      </c>
       <c r="I19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -12368,10 +12368,10 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D11" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -12379,10 +12379,10 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -12390,10 +12390,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D13" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12401,10 +12401,10 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12412,10 +12412,10 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -12423,10 +12423,10 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D16" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -12434,10 +12434,10 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -12445,10 +12445,10 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D18" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -12456,10 +12456,10 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -12882,7 +12882,7 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -12890,7 +12890,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -12898,7 +12898,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -12906,7 +12906,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -12914,7 +12914,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -12922,7 +12922,7 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
@@ -12930,7 +12930,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -12938,7 +12938,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -12946,7 +12946,7 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -13463,10 +13463,10 @@
         <v>125</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>125</v>
@@ -15926,7 +15926,7 @@
   <dimension ref="A1:J69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16224,22 +16224,22 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>250</v>
+        <v>456</v>
       </c>
       <c r="D15" t="s">
-        <v>250</v>
+        <v>456</v>
       </c>
       <c r="E15" t="s">
-        <v>250</v>
+        <v>456</v>
       </c>
       <c r="F15" t="s">
-        <v>250</v>
+        <v>456</v>
       </c>
       <c r="H15" t="s">
-        <v>250</v>
+        <v>456</v>
       </c>
       <c r="I15" t="s">
-        <v>250</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -16247,22 +16247,22 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -16270,22 +16270,22 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -16293,22 +16293,22 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -16316,22 +16316,22 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -16593,8 +16593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16698,7 +16698,7 @@
         <v>4.030671296296297E-3</v>
       </c>
       <c r="G3" s="3">
-        <v>3.7453703703703707E-3</v>
+        <v>4.4398148148148148E-3</v>
       </c>
       <c r="H3" s="3">
         <v>4.2187500000000003E-3</v>
@@ -16812,25 +16812,25 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I11" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -16838,25 +16838,25 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -16864,25 +16864,25 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -16890,25 +16890,25 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -16916,25 +16916,25 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -16942,25 +16942,25 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -16968,25 +16968,25 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I17" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -16994,25 +16994,25 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -17020,25 +17020,25 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -18107,19 +18107,19 @@
         <v>116</v>
       </c>
       <c r="C11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -18127,19 +18127,19 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
+        <v>269</v>
+      </c>
+      <c r="D12" t="s">
+        <v>269</v>
+      </c>
+      <c r="E12" t="s">
         <v>270</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>270</v>
       </c>
-      <c r="E12" t="s">
-        <v>271</v>
-      </c>
-      <c r="F12" t="s">
-        <v>271</v>
-      </c>
       <c r="G12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -18167,19 +18167,19 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D14" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E14" t="s">
+        <v>269</v>
+      </c>
+      <c r="F14" t="s">
+        <v>269</v>
+      </c>
+      <c r="G14" t="s">
         <v>270</v>
-      </c>
-      <c r="F14" t="s">
-        <v>270</v>
-      </c>
-      <c r="G14" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -18207,19 +18207,19 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -18227,19 +18227,19 @@
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G17" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -18247,19 +18247,19 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -18267,19 +18267,19 @@
         <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>